<commit_message>
Complete Lab Report 13
</commit_message>
<xml_diff>
--- a/Lab Reports/LabReport13/Lab 13 Excel.xlsx
+++ b/Lab Reports/LabReport13/Lab 13 Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NSFLab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abereni4u/Dropbox/Github/PHY121/Lab Reports/LabReport13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B061522-5D16-478C-832F-ACA86801B8B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE4CE55-EC02-0B4F-B6D4-0049A3221527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{DD142A35-FBF2-4062-9810-10A197F33D96}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12220" xr2:uid="{DD142A35-FBF2-4062-9810-10A197F33D96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,8 +57,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,8 +94,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,14 +127,47 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Part 1 - Spring Constant</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34269143234963012"/>
+          <c:y val="2.3809523809523808E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -129,7 +188,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -147,9 +206,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Weight</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -162,16 +218,128 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="88500"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="88500"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.5732527741817276E-2"/>
+                  <c:y val="-0.31929477565304337"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$11</c:f>
@@ -179,28 +347,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.49000000000000005</c:v>
+                  <c:v>2.0580000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98000000000000009</c:v>
+                  <c:v>2.5480000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.47</c:v>
+                  <c:v>3.0380000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9600000000000002</c:v>
+                  <c:v>3.528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>4.0180000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.94</c:v>
+                  <c:v>4.508</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.43</c:v>
+                  <c:v>4.9980000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9200000000000004</c:v>
+                  <c:v>5.4880000000000013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -212,28 +380,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.55500000000000005</c:v>
+                  <c:v>-0.55500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61499999999999999</c:v>
+                  <c:v>-0.61499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67500000000000004</c:v>
+                  <c:v>-0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73499999999999999</c:v>
+                  <c:v>-0.73499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79500000000000004</c:v>
+                  <c:v>-0.79500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.85499999999999998</c:v>
+                  <c:v>-0.85499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91500000000000004</c:v>
+                  <c:v>-0.91500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0149999999999999</c:v>
+                  <c:v>-1.0149999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -246,8 +414,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="b"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -278,6 +447,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Weight (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -291,14 +485,14 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -336,7 +530,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -369,6 +563,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Position (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -398,7 +647,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -449,7 +698,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr baseline="0">
+          <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -459,45 +710,33 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -1023,15 +1262,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1056,13 +1295,127 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>212933</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>106672</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>68442</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>81357</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Left Brace 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0175800D-E8F4-A523-1235-E8F732E35168}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6452013" y="1635886"/>
+          <a:ext cx="164805" cy="528533"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16597"/>
+            <a:gd name="adj2" fmla="val 48701"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.59661</cdr:x>
+      <cdr:y>0.29663</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.83258</cdr:x>
+      <cdr:y>0.37333</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4154E376-9B7A-8E71-09C8-2B3CBB813389}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3471474" y="957203"/>
+          <a:ext cx="1373070" cy="247517"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" kern="1200">
+              <a:latin typeface="LM Mono 10" pitchFamily="49" charset="77"/>
+            </a:rPr>
+            <a:t>Spring Constant</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1100,7 +1453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1206,7 +1559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1348,7 +1701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1356,132 +1709,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CCF436-5D29-4716-86CC-FBB01B34B070}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>0.05</v>
       </c>
-      <c r="B4">
-        <f>A4*9.8</f>
-        <v>0.49000000000000005</v>
-      </c>
-      <c r="C4">
-        <v>0.55500000000000005</v>
+      <c r="B4" s="1">
+        <f>(A4+A13)*9.8</f>
+        <v>2.0580000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-0.55500000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>0.1</v>
       </c>
-      <c r="B5">
-        <f t="shared" ref="B5:B11" si="0">A5*9.8</f>
-        <v>0.98000000000000009</v>
-      </c>
-      <c r="C5">
-        <v>0.61499999999999999</v>
+      <c r="B5" s="1">
+        <f>(A5+A13)*9.8</f>
+        <v>2.5480000000000005</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.61499999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>0.15</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1.47</v>
-      </c>
-      <c r="C6">
-        <v>0.67500000000000004</v>
+      <c r="B6" s="1">
+        <f>(A6+A13)*9.8</f>
+        <v>3.0380000000000003</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-0.67500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>0.2</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1.9600000000000002</v>
-      </c>
-      <c r="C7">
-        <v>0.73499999999999999</v>
+      <c r="B7" s="1">
+        <f>(A7+A13)*9.8</f>
+        <v>3.528</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-0.73499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>0.25</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C8">
-        <v>0.79500000000000004</v>
+      <c r="B8" s="1">
+        <f>(A8+A13)*9.8</f>
+        <v>4.0180000000000007</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-0.79500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>0.3</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>2.94</v>
-      </c>
-      <c r="C9">
-        <v>0.85499999999999998</v>
+      <c r="B9" s="1">
+        <f>(A9+A13)*9.8</f>
+        <v>4.508</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-0.85499999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>0.35</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>3.43</v>
-      </c>
-      <c r="C10">
-        <v>0.91500000000000004</v>
+      <c r="B10" s="1">
+        <f>(A10+A13)*9.8</f>
+        <v>4.9980000000000002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-0.91500000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>0.4</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3.9200000000000004</v>
-      </c>
-      <c r="C11">
-        <v>1.0149999999999999</v>
+      <c r="B11" s="1">
+        <f>(A11+A13)*9.8</f>
+        <v>5.4880000000000013</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-1.0149999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>